<commit_message>
literacy, 240930 modified 3
</commit_message>
<xml_diff>
--- a/R/data/quiz240923.xlsx
+++ b/R/data/quiz240923.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A4738C-7FD9-4248-A4EC-D246C225340A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EEA13E-3A19-A749-9276-19000C48DB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="48640" yWindow="4900" windowWidth="44800" windowHeight="22940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4593" uniqueCount="1041">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4813" uniqueCount="1084">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -3143,6 +3143,135 @@
   </si>
   <si>
     <t>유정현</t>
+  </si>
+  <si>
+    <t>whalsrl124@naver.com</t>
+  </si>
+  <si>
+    <t>조민기</t>
+  </si>
+  <si>
+    <t>ye1651@naver.com</t>
+  </si>
+  <si>
+    <t>전예은</t>
+  </si>
+  <si>
+    <t>wooyoomilk@naver.com</t>
+  </si>
+  <si>
+    <t>우연준</t>
+  </si>
+  <si>
+    <t>leejhzzang2005@naver.com</t>
+  </si>
+  <si>
+    <t>이주현</t>
+  </si>
+  <si>
+    <t>zzun1414@naver.com</t>
+  </si>
+  <si>
+    <t>반도체·디스플레이스쿨</t>
+  </si>
+  <si>
+    <t>황준영</t>
+  </si>
+  <si>
+    <t>qudcksl1216@gmail.com</t>
+  </si>
+  <si>
+    <t>윤병찬</t>
+  </si>
+  <si>
+    <t>kimdongx0813@gmail.com</t>
+  </si>
+  <si>
+    <t>2468pp@naver.com</t>
+  </si>
+  <si>
+    <t>박성빈</t>
+  </si>
+  <si>
+    <t>hihi2679@gmail.com</t>
+  </si>
+  <si>
+    <t>박서현</t>
+  </si>
+  <si>
+    <t>jerryterryharry@gmail.com</t>
+  </si>
+  <si>
+    <t>문진영</t>
+  </si>
+  <si>
+    <t>creeper_a@naver.com</t>
+  </si>
+  <si>
+    <t>최대현</t>
+  </si>
+  <si>
+    <t>h20202519@glab.hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>남현아</t>
+  </si>
+  <si>
+    <t>dawn2368@gmail.com</t>
+  </si>
+  <si>
+    <t>허다운</t>
+  </si>
+  <si>
+    <t>hjjj051014@naver.com</t>
+  </si>
+  <si>
+    <t>안효정</t>
+  </si>
+  <si>
+    <t>cmin0945@gmail.com</t>
+  </si>
+  <si>
+    <t>조상민</t>
+  </si>
+  <si>
+    <t>xogns3043@naver.com</t>
+  </si>
+  <si>
+    <t>김태훈</t>
+  </si>
+  <si>
+    <t>sbysoo@naver.com</t>
+  </si>
+  <si>
+    <t>신윤수</t>
+  </si>
+  <si>
+    <t>mingtto0920@gmail.com</t>
+  </si>
+  <si>
+    <t>유민서</t>
+  </si>
+  <si>
+    <t>leejs7807@gmail.com</t>
+  </si>
+  <si>
+    <t>이종선</t>
+  </si>
+  <si>
+    <t>jklucky09@naver.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">사회학과 </t>
+  </si>
+  <si>
+    <t>최준근</t>
+  </si>
+  <si>
+    <t>minwl19@naver.com</t>
+  </si>
+  <si>
+    <t>조민지</t>
   </si>
 </sst>
 </file>
@@ -3555,7 +3684,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:N459" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:N481" headerRowCount="0">
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
@@ -3782,11 +3911,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N459"/>
+  <dimension ref="A1:N481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A415" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F467" sqref="F467"/>
+      <pane ySplit="1" topLeftCell="A435" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E486" sqref="E486"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -22625,7 +22754,909 @@
       <c r="M459" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="N459" s="23"/>
+    </row>
+    <row r="460" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A460" s="4">
+        <v>45566.858015092592</v>
+      </c>
+      <c r="B460" s="5" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C460" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D460" s="5">
+        <v>20192986</v>
+      </c>
+      <c r="E460" s="5" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F460" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G460" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="H460" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I460" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J460" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K460" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L460" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N460" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="461" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A461" s="8">
+        <v>45566.865204664355</v>
+      </c>
+      <c r="B461" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C461" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D461" s="9">
+        <v>20243949</v>
+      </c>
+      <c r="E461" s="9" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F461" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G461" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="H461" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I461" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J461" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K461" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L461" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N461" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="462" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A462" s="4">
+        <v>45566.948050613428</v>
+      </c>
+      <c r="B462" s="5" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C462" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D462" s="5">
+        <v>20242988</v>
+      </c>
+      <c r="E462" s="5" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F462" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G462" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H462" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I462" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J462" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K462" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L462" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M462" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="463" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A463" s="8">
+        <v>45566.9987841088</v>
+      </c>
+      <c r="B463" s="9" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C463" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D463" s="9">
+        <v>20242342</v>
+      </c>
+      <c r="E463" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="F463" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G463" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="H463" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I463" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="J463" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K463" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L463" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M463" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="464" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A464" s="4">
+        <v>45567.089261122688</v>
+      </c>
+      <c r="B464" s="5" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C464" s="5" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D464" s="5">
+        <v>20203352</v>
+      </c>
+      <c r="E464" s="5" t="s">
+        <v>1051</v>
+      </c>
+      <c r="F464" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G464" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H464" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I464" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J464" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K464" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L464" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M464" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="465" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A465" s="8">
+        <v>45567.424144664357</v>
+      </c>
+      <c r="B465" s="9" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C465" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D465" s="9">
+        <v>20192926</v>
+      </c>
+      <c r="E465" s="9" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F465" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G465" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="H465" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I465" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J465" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K465" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L465" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M465" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="466" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A466" s="4">
+        <v>45567.474208530097</v>
+      </c>
+      <c r="B466" s="5" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C466" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D466" s="5">
+        <v>20182308</v>
+      </c>
+      <c r="E466" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="F466" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G466" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="H466" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I466" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J466" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K466" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L466" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N466" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="467" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A467" s="8">
+        <v>45567.545542557869</v>
+      </c>
+      <c r="B467" s="9" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C467" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D467" s="9">
+        <v>20193813</v>
+      </c>
+      <c r="E467" s="9" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F467" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G467" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="H467" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I467" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J467" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K467" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L467" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M467" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="468" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A468" s="4">
+        <v>45567.552172708332</v>
+      </c>
+      <c r="B468" s="5" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C468" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D468" s="5">
+        <v>20243815</v>
+      </c>
+      <c r="E468" s="5" t="s">
+        <v>1058</v>
+      </c>
+      <c r="F468" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G468" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H468" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I468" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J468" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K468" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L468" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M468" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="469" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A469" s="8">
+        <v>45567.555632280091</v>
+      </c>
+      <c r="B469" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="C469" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="D469" s="9">
+        <v>20227091</v>
+      </c>
+      <c r="E469" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="F469" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G469" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="H469" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I469" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J469" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K469" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L469" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M469" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="470" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A470" s="4">
+        <v>45567.636272071759</v>
+      </c>
+      <c r="B470" s="5" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C470" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D470" s="5">
+        <v>20205162</v>
+      </c>
+      <c r="E470" s="5" t="s">
+        <v>1060</v>
+      </c>
+      <c r="F470" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G470" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="H470" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I470" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J470" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K470" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L470" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M470" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="471" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A471" s="8">
+        <v>45567.653821481479</v>
+      </c>
+      <c r="B471" s="9" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C471" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D471" s="9">
+        <v>20194153</v>
+      </c>
+      <c r="E471" s="9" t="s">
+        <v>1062</v>
+      </c>
+      <c r="F471" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G471" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="H471" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I471" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J471" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K471" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L471" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N471" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="472" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A472" s="4">
+        <v>45567.673935798608</v>
+      </c>
+      <c r="B472" s="5" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C472" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="D472" s="5">
+        <v>20202519</v>
+      </c>
+      <c r="E472" s="5" t="s">
+        <v>1064</v>
+      </c>
+      <c r="F472" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G472" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H472" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I472" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J472" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K472" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L472" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M472" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="473" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A473" s="8">
+        <v>45567.678044166663</v>
+      </c>
+      <c r="B473" s="9" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C473" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D473" s="9">
+        <v>20197126</v>
+      </c>
+      <c r="E473" s="9" t="s">
+        <v>1066</v>
+      </c>
+      <c r="F473" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G473" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="H473" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I473" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J473" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K473" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L473" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M473" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="474" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A474" s="4">
+        <v>45567.688942962966</v>
+      </c>
+      <c r="B474" s="5" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C474" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="D474" s="5">
+        <v>20243628</v>
+      </c>
+      <c r="E474" s="5" t="s">
+        <v>1068</v>
+      </c>
+      <c r="F474" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G474" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="H474" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I474" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J474" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K474" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L474" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N474" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="475" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A475" s="15">
+        <v>45567.768053206019</v>
+      </c>
+      <c r="B475" s="16" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C475" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="D475" s="16">
+        <v>20246776</v>
+      </c>
+      <c r="E475" s="16" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F475" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G475" s="17">
+        <v>0.3</v>
+      </c>
+      <c r="H475" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="I475" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J475" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K475" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L475" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="M475" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="476" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A476" s="4">
+        <v>45567.810299409721</v>
+      </c>
+      <c r="B476" s="5" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C476" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="D476" s="5">
+        <v>20227040</v>
+      </c>
+      <c r="E476" s="5" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F476" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G476" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H476" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I476" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J476" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K476" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L476" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M476" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="477" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A477" s="8">
+        <v>45567.825215636578</v>
+      </c>
+      <c r="B477" s="9" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C477" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D477" s="9">
+        <v>20227155</v>
+      </c>
+      <c r="E477" s="9" t="s">
+        <v>1074</v>
+      </c>
+      <c r="F477" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G477" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="H477" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I477" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J477" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K477" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L477" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M477" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="478" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A478" s="4">
+        <v>45567.838763946755</v>
+      </c>
+      <c r="B478" s="5" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C478" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D478" s="5">
+        <v>20242540</v>
+      </c>
+      <c r="E478" s="5" t="s">
+        <v>1076</v>
+      </c>
+      <c r="F478" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G478" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="H478" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I478" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J478" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K478" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L478" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N478" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="479" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A479" s="8">
+        <v>45567.898840995374</v>
+      </c>
+      <c r="B479" s="9" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C479" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="D479" s="9">
+        <v>20223249</v>
+      </c>
+      <c r="E479" s="9" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F479" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G479" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="H479" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I479" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J479" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K479" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L479" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N479" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="480" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A480" s="4">
+        <v>45567.943901006947</v>
+      </c>
+      <c r="B480" s="5" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C480" s="5" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D480" s="5">
+        <v>20171101</v>
+      </c>
+      <c r="E480" s="5" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F480" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G480" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="H480" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I480" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J480" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K480" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L480" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M480" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="481" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A481" s="15">
+        <v>45568.057885648144</v>
+      </c>
+      <c r="B481" s="16" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C481" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="D481" s="16">
+        <v>20217178</v>
+      </c>
+      <c r="E481" s="16" t="s">
+        <v>1083</v>
+      </c>
+      <c r="F481" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G481" s="17">
+        <v>0.3</v>
+      </c>
+      <c r="H481" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="I481" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="J481" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K481" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L481" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M481" s="23"/>
+      <c r="N481" s="18" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>